<commit_message>
forced commit before pulling
</commit_message>
<xml_diff>
--- a/converting-test-cases.xlsx
+++ b/converting-test-cases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://seneca-my.sharepoint.com/personal/ldang15_myseneca_ca/Documents/CPRZII/final_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="85" documentId="13_ncr:1_{AF7501F5-17D9-44E9-B635-1D850C3927CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9B3EDD88-B5AC-4A3C-A4FF-5C120DA23317}"/>
+  <xr:revisionPtr revIDLastSave="87" documentId="13_ncr:1_{AF7501F5-17D9-44E9-B635-1D850C3927CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4A73A941-A8D7-4158-9ADB-3DBB258EE0FF}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1080" yWindow="1080" windowWidth="17280" windowHeight="8964" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="example to be deleted" sheetId="2" r:id="rId1"/>
@@ -1028,7 +1028,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="83">
   <si>
     <t>Program
 or module:</t>
@@ -1312,6 +1312,9 @@
   </si>
   <si>
     <t>The program does not handle strings longer than 16 char correctly</t>
+  </si>
+  <si>
+    <t>testing nomial function</t>
   </si>
 </sst>
 </file>
@@ -1842,6 +1845,30 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1853,30 +1880,6 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1945,6 +1948,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2236,22 +2243,22 @@
       <c r="B1" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="43" t="str">
+      <c r="C1" s="51" t="str">
         <f>"Do not save or use this worksheet – sample test cases only"</f>
         <v>Do not save or use this worksheet – sample test cases only</v>
       </c>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
     </row>
     <row r="2" spans="1:8" s="11" customFormat="1" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="42"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
       <c r="E2" s="29"/>
       <c r="F2" s="18" t="s">
         <v>3</v>
@@ -2441,8 +2448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{489FCF92-76BB-4101-9D49-11677A4362B7}">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2463,23 +2470,23 @@
       <c r="B1" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="C1" s="43" t="str">
+      <c r="C1" s="51" t="str">
         <f>"Save As " &amp; B1  &amp; "_test_cases.xlsx"</f>
         <v>Save As Converting_test_cases.xlsx</v>
       </c>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
     </row>
     <row r="2" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="42"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
       <c r="F2" s="20" t="s">
         <v>3</v>
       </c>
@@ -2523,7 +2530,7 @@
       <c r="D4" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="47" t="s">
+      <c r="E4" s="43" t="s">
         <v>45</v>
       </c>
       <c r="F4" s="10" t="s">
@@ -2546,7 +2553,7 @@
       <c r="D5" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="E5" s="47" t="s">
+      <c r="E5" s="43" t="s">
         <v>50</v>
       </c>
       <c r="F5" s="10" t="s">
@@ -2569,7 +2576,7 @@
       <c r="D6" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="E6" s="47" t="s">
+      <c r="E6" s="43" t="s">
         <v>45</v>
       </c>
       <c r="F6" s="10" t="s">
@@ -2592,7 +2599,7 @@
       <c r="D7" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="E7" s="47" t="s">
+      <c r="E7" s="43" t="s">
         <v>57</v>
       </c>
       <c r="F7" s="10" t="s">
@@ -2603,7 +2610,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A8" s="48" t="s">
+      <c r="A8" s="44" t="s">
         <v>37</v>
       </c>
       <c r="B8" s="24" t="s">
@@ -2618,15 +2625,15 @@
       <c r="E8" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="F8" s="49" t="s">
+      <c r="F8" s="45" t="s">
         <v>45</v>
       </c>
-      <c r="G8" s="50" t="s">
+      <c r="G8" s="46" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A9" s="48" t="s">
+      <c r="A9" s="44" t="s">
         <v>37</v>
       </c>
       <c r="B9" s="24" t="s">
@@ -2641,15 +2648,15 @@
       <c r="E9" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="F9" s="49" t="s">
+      <c r="F9" s="45" t="s">
         <v>45</v>
       </c>
-      <c r="G9" s="50" t="s">
+      <c r="G9" s="46" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="48" t="s">
+      <c r="A10" s="44" t="s">
         <v>37</v>
       </c>
       <c r="B10" s="24" t="s">
@@ -2664,10 +2671,10 @@
       <c r="E10" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="F10" s="49" t="s">
+      <c r="F10" s="45" t="s">
         <v>45</v>
       </c>
-      <c r="G10" s="50" t="s">
+      <c r="G10" s="46" t="s">
         <v>68</v>
       </c>
     </row>
@@ -2696,7 +2703,7 @@
     </row>
     <row r="12" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>37</v>
+        <v>82</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>38</v>
@@ -2707,13 +2714,13 @@
       <c r="D12" s="4">
         <v>1234.123</v>
       </c>
-      <c r="E12" s="46" t="s">
+      <c r="E12" s="42" t="s">
         <v>41</v>
       </c>
       <c r="F12" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="G12" s="45" t="s">
+      <c r="G12" s="41" t="s">
         <v>40</v>
       </c>
     </row>
@@ -2738,10 +2745,10 @@
       <c r="B14" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="C14" s="52" t="s">
+      <c r="C14" s="48" t="s">
         <v>73</v>
       </c>
-      <c r="D14" s="52" t="s">
+      <c r="D14" s="48" t="s">
         <v>75</v>
       </c>
       <c r="E14" s="3"/>
@@ -2754,13 +2761,13 @@
       <c r="B15" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="C15" s="51" t="s">
+      <c r="C15" s="47" t="s">
         <v>74</v>
       </c>
-      <c r="D15" s="51" t="s">
+      <c r="D15" s="47" t="s">
         <v>72</v>
       </c>
-      <c r="E15" s="51" t="s">
+      <c r="E15" s="47" t="s">
         <v>72</v>
       </c>
       <c r="F15" s="25" t="s">
@@ -2772,7 +2779,7 @@
     </row>
     <row r="16" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="26"/>
-      <c r="B16" s="51" t="s">
+      <c r="B16" s="47" t="s">
         <v>71</v>
       </c>
       <c r="C16" s="3" t="s">
@@ -2781,7 +2788,7 @@
       <c r="D16" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="E16" s="51" t="s">
+      <c r="E16" s="47" t="s">
         <v>77</v>
       </c>
       <c r="F16" s="25" t="s">
@@ -2790,7 +2797,7 @@
     </row>
     <row r="17" spans="1:7" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="26"/>
-      <c r="B17" s="51" t="s">
+      <c r="B17" s="47" t="s">
         <v>71</v>
       </c>
       <c r="C17" s="3" t="s">
@@ -2799,7 +2806,7 @@
       <c r="D17" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="E17" s="51" t="s">
+      <c r="E17" s="47" t="s">
         <v>77</v>
       </c>
       <c r="F17" s="25" t="s">
@@ -2807,13 +2814,13 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="41" t="s">
+      <c r="A18" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="42"/>
-      <c r="C18" s="42"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="42"/>
+      <c r="B18" s="50"/>
+      <c r="C18" s="50"/>
+      <c r="D18" s="50"/>
+      <c r="E18" s="50"/>
       <c r="F18" s="20" t="s">
         <v>3</v>
       </c>
@@ -2919,25 +2926,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="834b100a-dc26-4ede-9885-7b3df77c2ec4">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010041E2C5036B18264388124B3BD1005D20" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b8497cd80e96d74b5b6992e405b57094">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="834b100a-dc26-4ede-9885-7b3df77c2ec4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="059331ad37c3e30d81c2bb785f2f4871" ns2:_="">
     <xsd:import namespace="834b100a-dc26-4ede-9885-7b3df77c2ec4"/>
@@ -3103,10 +3091,39 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="834b100a-dc26-4ede-9885-7b3df77c2ec4">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69AA5A3E-E7E5-4059-8EBE-8A5728AA1F8C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FCB5079C-FEB5-44A1-9C3E-8CB7C2253050}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="834b100a-dc26-4ede-9885-7b3df77c2ec4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3122,19 +3139,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FCB5079C-FEB5-44A1-9C3E-8CB7C2253050}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69AA5A3E-E7E5-4059-8EBE-8A5728AA1F8C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="834b100a-dc26-4ede-9885-7b3df77c2ec4"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>